<commit_message>
template tag combine same attribute without underscore
</commit_message>
<xml_diff>
--- a/Raw Input Data/Template V2/SearchWarrant V2.xlsx
+++ b/Raw Input Data/Template V2/SearchWarrant V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Raw Input Data\Template V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D16E4AB-3E6C-4F58-9FF1-FADBEFC9E1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E95350-3352-40BF-9D4D-EF3FF947050E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="7" xr2:uid="{2E1C8D8E-ADF5-A447-A84C-DD0DD65940D4}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1268,8 +1268,8 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="str">
-        <f>'SearchWarrant-Template'!B6&amp;"&lt;u&gt;&lt;Template_Case_No&gt;"&amp;'SearchWarrant-Params'!B4&amp;"&lt;/Template_Case_No&gt;&lt;/u&gt;"</f>
-        <v>Case No. &lt;u&gt;&lt;Template_Case_No&gt;POLICEREF2&lt;/Template_Case_No&gt;&lt;/u&gt;</v>
+        <f>'SearchWarrant-Template'!B6&amp;"&lt;u&gt;&lt;Template_CaseNo&gt;"&amp;'SearchWarrant-Params'!B4&amp;"&lt;/Template_CaseNo&gt;&lt;/u&gt;"</f>
+        <v>Case No. &lt;u&gt;&lt;Template_CaseNo&gt;POLICEREF2&lt;/Template_CaseNo&gt;&lt;/u&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1280,8 +1280,8 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
-        <f>'SearchWarrant-Template'!B8&amp;"&lt;u&gt;&lt;Template_Writ_No&gt;"&amp;'SearchWarrant-Params'!B6&amp;"&lt;/Template_Writ_No&gt;&lt;/u&gt;"</f>
-        <v>Writ No. &lt;u&gt;&lt;Template_Writ_No&gt;TM ■■■■&lt;/Template_Writ_No&gt;&lt;/u&gt;</v>
+        <f>'SearchWarrant-Template'!B8&amp;"&lt;u&gt;&lt;Template_WritNo&gt;"&amp;'SearchWarrant-Params'!B6&amp;"&lt;/Template_WritNo&gt;&lt;/u&gt;"</f>
+        <v>Writ No. &lt;u&gt;&lt;Template_WritNo&gt;TM ■■■■&lt;/Template_WritNo&gt;&lt;/u&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1308,7 +1308,7 @@
         <v>**&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;**</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str" cm="1">
         <f t="array" ref="B9">"**&lt;u&gt;" &amp; _xlfn.LET(
   _xlpm.items,   _xlfn._xlws.FILTER('SearchWarrant-Requested-Items'!A2:A20, 'SearchWarrant-Requested-Items'!B2:B20="Y"),
@@ -1324,8 +1324,8 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
-        <f>"**&lt;u&gt;&lt;Template_Offence_Type&gt;"&amp;'SearchWarrant-Params'!B12&amp;"&lt;/Template_Offence_Type&gt;&lt;/u&gt;**"</f>
-        <v>**&lt;u&gt;&lt;Template_Offence_Type&gt;Obtaining Property By Deception, contrary to Section 17 (1 ) of the Theft Ordinance, Cap. 210, Laws of Hong Kong&lt;/Template_Offence_Type&gt;&lt;/u&gt;**</v>
+        <f>"**&lt;u&gt;&lt;Template_OffenceType&gt;"&amp;'SearchWarrant-Params'!B12&amp;"&lt;/Template_OffenceType&gt;&lt;/u&gt;**"</f>
+        <v>**&lt;u&gt;&lt;Template_OffenceType&gt;Obtaining Property By Deception, contrary to Section 17 (1 ) of the Theft Ordinance, Cap. 210, Laws of Hong Kong&lt;/Template_OffenceType&gt;&lt;/u&gt;**</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1564,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AFA931-1FCA-2846-9F01-97E33F78B0E2}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1587,8 +1587,8 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>'SearchWarrant-Template'!B4&amp;"&lt;Template_Contact_Person&gt;"&amp;'SearchWarrant-Params'!B2&amp;"&lt;/Template_Contact_Person&gt;"</f>
-        <v>Contact Person: &lt;Template_Contact_Person&gt;PC ■■■■■&lt;/Template_Contact_Person&gt;</v>
+        <f>'SearchWarrant-Template'!B4&amp;"&lt;Template_ContactPerson&gt;"&amp;'SearchWarrant-Params'!B2&amp;"&lt;/Template_ContactPerson&gt;"</f>
+        <v>Contact Person: &lt;Template_ContactPerson&gt;PC ■■■■■&lt;/Template_ContactPerson&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -1600,7 +1600,7 @@
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>'SearchWarrant-Runtime-Params'!B2</f>
-        <v>Case No. &lt;u&gt;&lt;Template_Case_No&gt;POLICEREF2&lt;/Template_Case_No&gt;&lt;/u&gt;</v>
+        <v>Case No. &lt;u&gt;&lt;Template_CaseNo&gt;POLICEREF2&lt;/Template_CaseNo&gt;&lt;/u&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>'SearchWarrant-Runtime-Params'!B4</f>
-        <v>Writ No. &lt;u&gt;&lt;Template_Writ_No&gt;TM ■■■■&lt;/Template_Writ_No&gt;&lt;/u&gt;</v>
+        <v>Writ No. &lt;u&gt;&lt;Template_WritNo&gt;TM ■■■■&lt;/Template_WritNo&gt;&lt;/u&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -1636,10 +1636,10 @@
     <row r="15" spans="1:1" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>'SearchWarrant-Template'!B13&amp;'SearchWarrant-Runtime-Params'!B6&amp;'SearchWarrant-Template'!B14&amp;'SearchWarrant-Runtime-Params'!B7&amp;'SearchWarrant-Template'!B15&amp;'SearchWarrant-Runtime-Params'!B8&amp;'SearchWarrant-Template'!B16&amp;'SearchWarrant-Runtime-Params'!B9&amp;'SearchWarrant-Template'!B17&amp;'SearchWarrant-Runtime-Params'!B10&amp;'SearchWarrant-Template'!B18&amp;'SearchWarrant-Runtime-Params'!B11&amp;"."</f>
-        <v>INFORMATION has this day been laid before the undersigned, a magistrate of Hong Kong, on oath by **&lt;u&gt;&lt;Template_Deponent&gt;Detective Police Constable 2■■■■ LO ■■■■-■■ of DistrictInvestigation Team 4 Tuen Mun District, New Territories North&lt;/Template_Deponent&gt;&lt;/u&gt;**, that there is reasonable cause to suspect that there is in a building or place, namely, **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** certain books or other documents, or any portion or extract therefrom, or any other article, namely, **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_Requested_Account_Number&gt;111-111111-101&lt;/Template_Requested_Account_Number&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which are likely to be of value (whether by itself or together with anything else) to the investigation of an offence, namely, **&lt;u&gt;&lt;Template_Offence_Type&gt;Obtaining Property By Deception, contrary to Section 17 (1 ) of the Theft Ordinance, Cap. 210, Laws of Hong Kong&lt;/Template_Offence_Type&gt;&lt;/u&gt;** that has been committed or that is reasonably suspected ~~has been committed/~~ is reasonably to have been commited ~~/to be about to be committed/to be intended to be committed~~.</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="189" x14ac:dyDescent="0.25">
+        <v>INFORMATION has this day been laid before the undersigned, a magistrate of Hong Kong, on oath by **&lt;u&gt;&lt;Template_Deponent&gt;Detective Police Constable 2■■■■ LO ■■■■-■■ of DistrictInvestigation Team 4 Tuen Mun District, New Territories North&lt;/Template_Deponent&gt;&lt;/u&gt;**, that there is reasonable cause to suspect that there is in a building or place, namely, **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** certain books or other documents, or any portion or extract therefrom, or any other article, namely, **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_Requested_Account_Number&gt;111-111111-101&lt;/Template_Requested_Account_Number&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which are likely to be of value (whether by itself or together with anything else) to the investigation of an offence, namely, **&lt;u&gt;&lt;Template_OffenceType&gt;Obtaining Property By Deception, contrary to Section 17 (1 ) of the Theft Ordinance, Cap. 210, Laws of Hong Kong&lt;/Template_OffenceType&gt;&lt;/u&gt;** that has been committed or that is reasonably suspected ~~has been committed/~~ is reasonably to have been commited ~~/to be about to be committed/to be intended to be committed~~.</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>'SearchWarrant-Runtime-Params'!B12&amp;'SearchWarrant-Runtime-Params'!B7&amp;'SearchWarrant-Template'!B15&amp;'SearchWarrant-Runtime-Params'!B8&amp;'SearchWarrant-Template'!B22&amp;'SearchWarrant-Runtime-Params'!B9&amp;'SearchWarrant-Template'!B23&amp;'SearchWarrant-Runtime-Params'!B13</f>
         <v>You are herewith empowered to enter ~~and if necessary to break into or forcibly enter~~ the said building or place, namely **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** and to search for and take possession of the said books or other documents or portion of or extract therefrom or any other article, namely **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_Requested_Account_Number&gt;111-111111-101&lt;/Template_Requested_Account_Number&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which may be found therein; ~~and to detain during such period as is reasonably required to permit such a search to be carried out, any person who may appear to have such book or other document or portion thereof or extract therefrom or other article in his possession or under his control and who, if not so detained, might prejudice the purpose of the search.~~</v>

</xml_diff>

<commit_message>
fix missing template tag
</commit_message>
<xml_diff>
--- a/Raw Input Data/Template V2/SearchWarrant V2.xlsx
+++ b/Raw Input Data/Template V2/SearchWarrant V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Raw Input Data\Template V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E95350-3352-40BF-9D4D-EF3FF947050E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A9F1D1-FB60-4215-AA89-3042541D1212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="7" xr2:uid="{2E1C8D8E-ADF5-A447-A84C-DD0DD65940D4}"/>
+    <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="5" xr2:uid="{2E1C8D8E-ADF5-A447-A84C-DD0DD65940D4}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchWarrant-Params" sheetId="3" r:id="rId1"/>
@@ -1248,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39BF623-D88F-674B-A582-2932D90716E2}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1315,11 +1315,11 @@
   _xlpm.remarks, _xlfn._xlws.FILTER('SearchWarrant-Requested-Items'!C2:C20, 'SearchWarrant-Requested-Items'!B2:B20="Y"),
   _xlpm.ct,      ROWS(_xlpm.items),
   _xlpm.numbering, "(" &amp; _xlfn.SEQUENCE(_xlpm.ct, 1, 1, 1) &amp; ") ",
-  _xlpm.combined, _xlpm.items &amp; IF(_xlpm.remarks&lt;&gt;"", " " &amp;"&lt;Template_Requested_Account_Number&gt;" &amp; _xlpm.remarks &amp; "&lt;/Template_Requested_Account_Number&gt;", ""),
+  _xlpm.combined, _xlpm.items &amp; IF(_xlpm.remarks&lt;&gt;"", " " &amp;"&lt;Template_RequestedAccountNumber&gt;" &amp; _xlpm.remarks &amp; "&lt;/Template_RequestedAccountNumber&gt;", ""),
   _xlpm.textOut, _xlpm.numbering &amp; _xlpm.combined,
   _xlfn.TEXTJOIN(" ", TRUE, _xlpm.textOut)
 ) &amp; "&lt;/u&gt;**"</f>
-        <v>**&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_Requested_Account_Number&gt;111-111111-101&lt;/Template_Requested_Account_Number&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;**</v>
+        <v>**&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_RequestedAccountNumber&gt;111-111111-101&lt;/Template_RequestedAccountNumber&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;**</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1564,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AFA931-1FCA-2846-9F01-97E33F78B0E2}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1636,13 +1636,13 @@
     <row r="15" spans="1:1" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>'SearchWarrant-Template'!B13&amp;'SearchWarrant-Runtime-Params'!B6&amp;'SearchWarrant-Template'!B14&amp;'SearchWarrant-Runtime-Params'!B7&amp;'SearchWarrant-Template'!B15&amp;'SearchWarrant-Runtime-Params'!B8&amp;'SearchWarrant-Template'!B16&amp;'SearchWarrant-Runtime-Params'!B9&amp;'SearchWarrant-Template'!B17&amp;'SearchWarrant-Runtime-Params'!B10&amp;'SearchWarrant-Template'!B18&amp;'SearchWarrant-Runtime-Params'!B11&amp;"."</f>
-        <v>INFORMATION has this day been laid before the undersigned, a magistrate of Hong Kong, on oath by **&lt;u&gt;&lt;Template_Deponent&gt;Detective Police Constable 2■■■■ LO ■■■■-■■ of DistrictInvestigation Team 4 Tuen Mun District, New Territories North&lt;/Template_Deponent&gt;&lt;/u&gt;**, that there is reasonable cause to suspect that there is in a building or place, namely, **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** certain books or other documents, or any portion or extract therefrom, or any other article, namely, **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_Requested_Account_Number&gt;111-111111-101&lt;/Template_Requested_Account_Number&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which are likely to be of value (whether by itself or together with anything else) to the investigation of an offence, namely, **&lt;u&gt;&lt;Template_OffenceType&gt;Obtaining Property By Deception, contrary to Section 17 (1 ) of the Theft Ordinance, Cap. 210, Laws of Hong Kong&lt;/Template_OffenceType&gt;&lt;/u&gt;** that has been committed or that is reasonably suspected ~~has been committed/~~ is reasonably to have been commited ~~/to be about to be committed/to be intended to be committed~~.</v>
+        <v>INFORMATION has this day been laid before the undersigned, a magistrate of Hong Kong, on oath by **&lt;u&gt;&lt;Template_Deponent&gt;Detective Police Constable 2■■■■ LO ■■■■-■■ of DistrictInvestigation Team 4 Tuen Mun District, New Territories North&lt;/Template_Deponent&gt;&lt;/u&gt;**, that there is reasonable cause to suspect that there is in a building or place, namely, **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** certain books or other documents, or any portion or extract therefrom, or any other article, namely, **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_RequestedAccountNumber&gt;111-111111-101&lt;/Template_RequestedAccountNumber&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which are likely to be of value (whether by itself or together with anything else) to the investigation of an offence, namely, **&lt;u&gt;&lt;Template_OffenceType&gt;Obtaining Property By Deception, contrary to Section 17 (1 ) of the Theft Ordinance, Cap. 210, Laws of Hong Kong&lt;/Template_OffenceType&gt;&lt;/u&gt;** that has been committed or that is reasonably suspected ~~has been committed/~~ is reasonably to have been commited ~~/to be about to be committed/to be intended to be committed~~.</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>'SearchWarrant-Runtime-Params'!B12&amp;'SearchWarrant-Runtime-Params'!B7&amp;'SearchWarrant-Template'!B15&amp;'SearchWarrant-Runtime-Params'!B8&amp;'SearchWarrant-Template'!B22&amp;'SearchWarrant-Runtime-Params'!B9&amp;'SearchWarrant-Template'!B23&amp;'SearchWarrant-Runtime-Params'!B13</f>
-        <v>You are herewith empowered to enter ~~and if necessary to break into or forcibly enter~~ the said building or place, namely **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** and to search for and take possession of the said books or other documents or portion of or extract therefrom or any other article, namely **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_Requested_Account_Number&gt;111-111111-101&lt;/Template_Requested_Account_Number&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which may be found therein; ~~and to detain during such period as is reasonably required to permit such a search to be carried out, any person who may appear to have such book or other document or portion thereof or extract therefrom or other article in his possession or under his control and who, if not so detained, might prejudice the purpose of the search.~~</v>
+        <v>You are herewith empowered to enter ~~and if necessary to break into or forcibly enter~~ the said building or place, namely **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** and to search for and take possession of the said books or other documents or portion of or extract therefrom or any other article, namely **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_RequestedAccountNumber&gt;111-111111-101&lt;/Template_RequestedAccountNumber&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which may be found therein; ~~and to detain during such period as is reasonably required to permit such a search to be carried out, any person who may appear to have such book or other document or portion thereof or extract therefrom or other article in his possession or under his control and who, if not so detained, might prejudice the purpose of the search.~~</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change requested account number to suspect # account number
</commit_message>
<xml_diff>
--- a/Raw Input Data/Template V2/SearchWarrant V2.xlsx
+++ b/Raw Input Data/Template V2/SearchWarrant V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Raw Input Data\Template V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A9F1D1-FB60-4215-AA89-3042541D1212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B04848C-86FC-4629-B820-979BC80F7EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="5" xr2:uid="{2E1C8D8E-ADF5-A447-A84C-DD0DD65940D4}"/>
+    <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" tabRatio="769" firstSheet="1" activeTab="5" xr2:uid="{2E1C8D8E-ADF5-A447-A84C-DD0DD65940D4}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchWarrant-Params" sheetId="3" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
   <si>
     <t>Template_Var</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>Raymond</t>
+  </si>
+  <si>
+    <t>Suspect Number</t>
   </si>
 </sst>
 </file>
@@ -1092,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B4D2FA-20FE-E543-BD9F-914FDC417667}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1104,7 +1107,7 @@
     <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1114,8 +1117,11 @@
       <c r="C1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -1125,8 +1131,11 @@
       <c r="C2" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1134,7 +1143,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -1142,7 +1151,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1248,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39BF623-D88F-674B-A582-2932D90716E2}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1313,13 +1322,14 @@
         <f t="array" ref="B9">"**&lt;u&gt;" &amp; _xlfn.LET(
   _xlpm.items,   _xlfn._xlws.FILTER('SearchWarrant-Requested-Items'!A2:A20, 'SearchWarrant-Requested-Items'!B2:B20="Y"),
   _xlpm.remarks, _xlfn._xlws.FILTER('SearchWarrant-Requested-Items'!C2:C20, 'SearchWarrant-Requested-Items'!B2:B20="Y"),
+  _xlpm.suspectNumber, _xlfn._xlws.FILTER('SearchWarrant-Requested-Items'!D2:D20, 'SearchWarrant-Requested-Items'!B2:B20="Y"),
   _xlpm.ct,      ROWS(_xlpm.items),
   _xlpm.numbering, "(" &amp; _xlfn.SEQUENCE(_xlpm.ct, 1, 1, 1) &amp; ") ",
-  _xlpm.combined, _xlpm.items &amp; IF(_xlpm.remarks&lt;&gt;"", " " &amp;"&lt;Template_RequestedAccountNumber&gt;" &amp; _xlpm.remarks &amp; "&lt;/Template_RequestedAccountNumber&gt;", ""),
+  _xlpm.combined, _xlpm.items &amp; IF(_xlpm.remarks&lt;&gt;"", " " &amp;"&lt;Template_Suspect"&amp;_xlpm.suspectNumber&amp;"_AccountNumber&gt;" &amp; _xlpm.remarks &amp; "&lt;/Template_Suspect"&amp;_xlpm.suspectNumber&amp;"_AccountNumber&gt;", ""),
   _xlpm.textOut, _xlpm.numbering &amp; _xlpm.combined,
   _xlfn.TEXTJOIN(" ", TRUE, _xlpm.textOut)
 ) &amp; "&lt;/u&gt;**"</f>
-        <v>**&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_RequestedAccountNumber&gt;111-111111-101&lt;/Template_RequestedAccountNumber&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;**</v>
+        <v>**&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_Suspect1_AccountNumber&gt;111-111111-101&lt;/Template_Suspect1_AccountNumber&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;**</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1392,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E096B48-7A56-3547-A897-287ED2A038D8}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1565,7 +1575,7 @@
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1636,13 +1646,13 @@
     <row r="15" spans="1:1" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>'SearchWarrant-Template'!B13&amp;'SearchWarrant-Runtime-Params'!B6&amp;'SearchWarrant-Template'!B14&amp;'SearchWarrant-Runtime-Params'!B7&amp;'SearchWarrant-Template'!B15&amp;'SearchWarrant-Runtime-Params'!B8&amp;'SearchWarrant-Template'!B16&amp;'SearchWarrant-Runtime-Params'!B9&amp;'SearchWarrant-Template'!B17&amp;'SearchWarrant-Runtime-Params'!B10&amp;'SearchWarrant-Template'!B18&amp;'SearchWarrant-Runtime-Params'!B11&amp;"."</f>
-        <v>INFORMATION has this day been laid before the undersigned, a magistrate of Hong Kong, on oath by **&lt;u&gt;&lt;Template_Deponent&gt;Detective Police Constable 2■■■■ LO ■■■■-■■ of DistrictInvestigation Team 4 Tuen Mun District, New Territories North&lt;/Template_Deponent&gt;&lt;/u&gt;**, that there is reasonable cause to suspect that there is in a building or place, namely, **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** certain books or other documents, or any portion or extract therefrom, or any other article, namely, **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_RequestedAccountNumber&gt;111-111111-101&lt;/Template_RequestedAccountNumber&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which are likely to be of value (whether by itself or together with anything else) to the investigation of an offence, namely, **&lt;u&gt;&lt;Template_OffenceType&gt;Obtaining Property By Deception, contrary to Section 17 (1 ) of the Theft Ordinance, Cap. 210, Laws of Hong Kong&lt;/Template_OffenceType&gt;&lt;/u&gt;** that has been committed or that is reasonably suspected ~~has been committed/~~ is reasonably to have been commited ~~/to be about to be committed/to be intended to be committed~~.</v>
+        <v>INFORMATION has this day been laid before the undersigned, a magistrate of Hong Kong, on oath by **&lt;u&gt;&lt;Template_Deponent&gt;Detective Police Constable 2■■■■ LO ■■■■-■■ of DistrictInvestigation Team 4 Tuen Mun District, New Territories North&lt;/Template_Deponent&gt;&lt;/u&gt;**, that there is reasonable cause to suspect that there is in a building or place, namely, **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** certain books or other documents, or any portion or extract therefrom, or any other article, namely, **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_Suspect1_AccountNumber&gt;111-111111-101&lt;/Template_Suspect1_AccountNumber&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which are likely to be of value (whether by itself or together with anything else) to the investigation of an offence, namely, **&lt;u&gt;&lt;Template_OffenceType&gt;Obtaining Property By Deception, contrary to Section 17 (1 ) of the Theft Ordinance, Cap. 210, Laws of Hong Kong&lt;/Template_OffenceType&gt;&lt;/u&gt;** that has been committed or that is reasonably suspected ~~has been committed/~~ is reasonably to have been commited ~~/to be about to be committed/to be intended to be committed~~.</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>'SearchWarrant-Runtime-Params'!B12&amp;'SearchWarrant-Runtime-Params'!B7&amp;'SearchWarrant-Template'!B15&amp;'SearchWarrant-Runtime-Params'!B8&amp;'SearchWarrant-Template'!B22&amp;'SearchWarrant-Runtime-Params'!B9&amp;'SearchWarrant-Template'!B23&amp;'SearchWarrant-Runtime-Params'!B13</f>
-        <v>You are herewith empowered to enter ~~and if necessary to break into or forcibly enter~~ the said building or place, namely **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** and to search for and take possession of the said books or other documents or portion of or extract therefrom or any other article, namely **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_RequestedAccountNumber&gt;111-111111-101&lt;/Template_RequestedAccountNumber&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which may be found therein; ~~and to detain during such period as is reasonably required to permit such a search to be carried out, any person who may appear to have such book or other document or portion thereof or extract therefrom or other article in his possession or under his control and who, if not so detained, might prejudice the purpose of the search.~~</v>
+        <v>You are herewith empowered to enter ~~and if necessary to break into or forcibly enter~~ the said building or place, namely **&lt;u&gt;Hang Seng Bank Limited&lt;/u&gt;** and situated at **&lt;u&gt;AML - Financial Crime Compliance, 8/F, Hang Seng 113, 113 Argyle Street, Mongkok, Kowloon, Hong Kong&lt;/u&gt;** and to search for and take possession of the said books or other documents or portion of or extract therefrom or any other article, namely **&lt;u&gt;(1) the opening mandates &amp; personal identity documents of bank accounts no.:  &lt;Template_Suspect1_AccountNumber&gt;111-111111-101&lt;/Template_Suspect1_AccountNumber&gt; (2) the above mentioned accounts transaction record from opening date to present, (3) all the swift message/ voucher,&lt;/u&gt;** which may be found therein; ~~and to detain during such period as is reasonably required to permit such a search to be carried out, any person who may appear to have such book or other document or portion thereof or extract therefrom or other article in his possession or under his control and who, if not so detained, might prejudice the purpose of the search.~~</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>